<commit_message>
Fix i2c (issue #48)
* lower R48 to 2k2
* connect IC10 directly to EEM0_I2C (before T6, T9)
* connect IC10 and config pins to P3V3_MP
</commit_message>
<xml_diff>
--- a/SIM_CALC/Fastino_Power_Budget.xlsx
+++ b/SIM_CALC/Fastino_Power_Budget.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\DESIGNS\Sinara_ALTIUM\EEMs\Fastino\SIM_CALC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hardware\Fastino\SIM_CALC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D787C-6A4B-44E2-8065-070972BD9481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DC8AE76-D61D-429B-865D-84EDF473E4BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -572,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C130ADAE-2F1D-4FBF-B703-EFB3430E5979}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,8 +741,11 @@
         <v>16</v>
       </c>
       <c r="F13">
-        <f>12*2</f>
-        <v>24</v>
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -852,7 +854,7 @@
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="F29">
+      <c r="L29">
         <v>20</v>
       </c>
     </row>
@@ -886,7 +888,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>346.1</v>
+        <v>314.10000000000002</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
@@ -910,7 +912,7 @@
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="M32">
         <f t="shared" si="0"/>
@@ -968,7 +970,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>510.82727272727277</v>
+        <v>478.82727272727277</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -992,7 +994,7 @@
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="M34">
         <f t="shared" si="1"/>
@@ -1025,7 +1027,7 @@
       </c>
       <c r="F35">
         <f>F34*3.3</f>
-        <v>1685.73</v>
+        <v>1580.13</v>
       </c>
       <c r="G35">
         <f>G34*5.4</f>
@@ -1049,7 +1051,7 @@
       </c>
       <c r="L35">
         <f>L34*3.3</f>
-        <v>9.8999999999999986</v>
+        <v>115.5</v>
       </c>
       <c r="M35">
         <f>M34*13</f>
@@ -1130,7 +1132,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>168.57299999999995</v>
+        <v>158.01299999999998</v>
       </c>
       <c r="G37">
         <f t="shared" si="2"/>
@@ -1154,7 +1156,7 @@
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
-        <v>9.8999999999999986</v>
+        <v>115.5</v>
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
@@ -1166,7 +1168,7 @@
       </c>
       <c r="O37">
         <f>SUM(B37:N37)</f>
-        <v>3221.8887076923074</v>
+        <v>3316.9287076923069</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,7 +1185,7 @@
       </c>
       <c r="F40">
         <f>F35</f>
-        <v>1685.73</v>
+        <v>1580.13</v>
       </c>
       <c r="H40">
         <f>H35</f>
@@ -1199,7 +1201,7 @@
       </c>
       <c r="O40">
         <f>SUM(B40:N40)+O37</f>
-        <v>16821.198707692307</v>
+        <v>16810.638707692306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1 fixes by @pathfinder49
</commit_message>
<xml_diff>
--- a/SIM_CALC/Fastino_Power_Budget.xlsx
+++ b/SIM_CALC/Fastino_Power_Budget.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\DESIGNS\Sinara_ALTIUM\EEMs\Fastino\SIM_CALC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hardware\Fastino\SIM_CALC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D787C-6A4B-44E2-8065-070972BD9481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DC8AE76-D61D-429B-865D-84EDF473E4BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -572,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C130ADAE-2F1D-4FBF-B703-EFB3430E5979}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,8 +741,11 @@
         <v>16</v>
       </c>
       <c r="F13">
-        <f>12*2</f>
-        <v>24</v>
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -852,7 +854,7 @@
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="F29">
+      <c r="L29">
         <v>20</v>
       </c>
     </row>
@@ -886,7 +888,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>346.1</v>
+        <v>314.10000000000002</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
@@ -910,7 +912,7 @@
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="M32">
         <f t="shared" si="0"/>
@@ -968,7 +970,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>510.82727272727277</v>
+        <v>478.82727272727277</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -992,7 +994,7 @@
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="M34">
         <f t="shared" si="1"/>
@@ -1025,7 +1027,7 @@
       </c>
       <c r="F35">
         <f>F34*3.3</f>
-        <v>1685.73</v>
+        <v>1580.13</v>
       </c>
       <c r="G35">
         <f>G34*5.4</f>
@@ -1049,7 +1051,7 @@
       </c>
       <c r="L35">
         <f>L34*3.3</f>
-        <v>9.8999999999999986</v>
+        <v>115.5</v>
       </c>
       <c r="M35">
         <f>M34*13</f>
@@ -1130,7 +1132,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>168.57299999999995</v>
+        <v>158.01299999999998</v>
       </c>
       <c r="G37">
         <f t="shared" si="2"/>
@@ -1154,7 +1156,7 @@
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
-        <v>9.8999999999999986</v>
+        <v>115.5</v>
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
@@ -1166,7 +1168,7 @@
       </c>
       <c r="O37">
         <f>SUM(B37:N37)</f>
-        <v>3221.8887076923074</v>
+        <v>3316.9287076923069</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,7 +1185,7 @@
       </c>
       <c r="F40">
         <f>F35</f>
-        <v>1685.73</v>
+        <v>1580.13</v>
       </c>
       <c r="H40">
         <f>H35</f>
@@ -1199,7 +1201,7 @@
       </c>
       <c r="O40">
         <f>SUM(B40:N40)+O37</f>
-        <v>16821.198707692307</v>
+        <v>16810.638707692306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>